<commit_message>
updated datasets v9 with corrected Ewald energy calculation
</commit_message>
<xml_diff>
--- a/data/processed/IMT_Classification_Dataset_Reduced_Feature_Set_v9.xlsx
+++ b/data/processed/IMT_Classification_Dataset_Reduced_Feature_Set_v9.xlsx
@@ -467,7 +467,7 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>ewald_energy</t>
+          <t>ewald_energy_per_atom</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -525,7 +525,7 @@
         <v>11.9464264123988</v>
       </c>
       <c r="G2" t="n">
-        <v>-176.4374920521197</v>
+        <v>-35.28749841042394</v>
       </c>
       <c r="H2" t="n">
         <v>87</v>
@@ -570,7 +570,7 @@
         <v>21.59576622103683</v>
       </c>
       <c r="G3" t="n">
-        <v>-147.2111445465009</v>
+        <v>-18.40139306831261</v>
       </c>
       <c r="H3" t="n">
         <v>88</v>
@@ -615,7 +615,7 @@
         <v>3.591514787961472</v>
       </c>
       <c r="G4" t="n">
-        <v>-1467.306977241031</v>
+        <v>-32.60682171646735</v>
       </c>
       <c r="H4" t="n">
         <v>87</v>
@@ -660,7 +660,7 @@
         <v>11.8761415231632</v>
       </c>
       <c r="G5" t="n">
-        <v>-3513.136460690042</v>
+        <v>-39.92200523511411</v>
       </c>
       <c r="H5" t="n">
         <v>87</v>
@@ -705,7 +705,7 @@
         <v>8.827433771370124</v>
       </c>
       <c r="G6" t="n">
-        <v>-1622.921775965516</v>
+        <v>-33.81087033261491</v>
       </c>
       <c r="H6" t="n">
         <v>87</v>
@@ -750,7 +750,7 @@
         <v>7.076892085048883</v>
       </c>
       <c r="G7" t="n">
-        <v>-755.3108971846848</v>
+        <v>-37.76554485923424</v>
       </c>
       <c r="H7" t="n">
         <v>87</v>
@@ -795,7 +795,7 @@
         <v>12.71527035222468</v>
       </c>
       <c r="G8" t="n">
-        <v>-722.3895826149167</v>
+        <v>-36.11947913074583</v>
       </c>
       <c r="H8" t="n">
         <v>87</v>
@@ -840,7 +840,7 @@
         <v>11.70196161966729</v>
       </c>
       <c r="G9" t="n">
-        <v>-733.0799077219642</v>
+        <v>-36.65399538609821</v>
       </c>
       <c r="H9" t="n">
         <v>87</v>
@@ -885,7 +885,7 @@
         <v>8.219416899913824</v>
       </c>
       <c r="G10" t="n">
-        <v>-290.6597180876894</v>
+        <v>-48.44328634794823</v>
       </c>
       <c r="H10" t="n">
         <v>87</v>
@@ -930,7 +930,7 @@
         <v>14.84247793525028</v>
       </c>
       <c r="G11" t="n">
-        <v>-279.3134636522442</v>
+        <v>-46.5522439420407</v>
       </c>
       <c r="H11" t="n">
         <v>87</v>
@@ -975,7 +975,7 @@
         <v>8.357028110579</v>
       </c>
       <c r="G12" t="n">
-        <v>-995.8900320189128</v>
+        <v>-33.19633440063043</v>
       </c>
       <c r="H12" t="n">
         <v>87</v>
@@ -1020,7 +1020,7 @@
         <v>10.54882687841495</v>
       </c>
       <c r="G13" t="n">
-        <v>-1005.984269434909</v>
+        <v>-33.53280898116362</v>
       </c>
       <c r="H13" t="n">
         <v>87</v>
@@ -1065,7 +1065,7 @@
         <v>14.90462245861747</v>
       </c>
       <c r="G14" t="n">
-        <v>-650.5000523175408</v>
+        <v>-32.52500261587704</v>
       </c>
       <c r="H14" t="n">
         <v>87</v>
@@ -1110,7 +1110,7 @@
         <v>13.71425218019586</v>
       </c>
       <c r="G15" t="n">
-        <v>-483.5273113429531</v>
+        <v>-30.22045695893457</v>
       </c>
       <c r="H15" t="n">
         <v>87</v>
@@ -1155,7 +1155,7 @@
         <v>13.60238430793818</v>
       </c>
       <c r="G16" t="n">
-        <v>-541.2808424889038</v>
+        <v>-45.10673687407532</v>
       </c>
       <c r="H16" t="n">
         <v>87</v>
@@ -1200,7 +1200,7 @@
         <v>12.27600804284653</v>
       </c>
       <c r="G17" t="n">
-        <v>-123.4384878599528</v>
+        <v>-20.57308130999214</v>
       </c>
       <c r="H17" t="n">
         <v>87</v>
@@ -1245,7 +1245,7 @@
         <v>13.6870525618895</v>
       </c>
       <c r="G18" t="n">
-        <v>-278.6319689063139</v>
+        <v>-46.43866148438565</v>
       </c>
       <c r="H18" t="n">
         <v>87</v>
@@ -1290,7 +1290,7 @@
         <v>14.82768992180982</v>
       </c>
       <c r="G19" t="n">
-        <v>-275.5834115789704</v>
+        <v>-45.93056859649506</v>
       </c>
       <c r="H19" t="n">
         <v>87</v>
@@ -1335,7 +1335,7 @@
         <v>9.286902256504558</v>
       </c>
       <c r="G20" t="n">
-        <v>-275.0245679997435</v>
+        <v>-68.75614199993588</v>
       </c>
       <c r="H20" t="n">
         <v>87</v>
@@ -1380,7 +1380,7 @@
         <v>13.84601722061992</v>
       </c>
       <c r="G21" t="n">
-        <v>-283.4275860525534</v>
+        <v>-47.2379310087589</v>
       </c>
       <c r="H21" t="n">
         <v>87</v>
@@ -1425,7 +1425,7 @@
         <v>7.310726177978318</v>
       </c>
       <c r="G22" t="n">
-        <v>-3355.338257723023</v>
+        <v>-39.94450306813123</v>
       </c>
       <c r="H22" t="n">
         <v>87</v>
@@ -1470,7 +1470,7 @@
         <v>10.33471514566295</v>
       </c>
       <c r="G23" t="n">
-        <v>-281.5246937512252</v>
+        <v>-46.92078229187086</v>
       </c>
       <c r="H23" t="n">
         <v>87</v>
@@ -1515,7 +1515,7 @@
         <v>13.20280535268414</v>
       </c>
       <c r="G24" t="n">
-        <v>-431.6313451757958</v>
+        <v>-30.8308103696997</v>
       </c>
       <c r="H24" t="n">
         <v>87</v>
@@ -1560,7 +1560,7 @@
         <v>9.681410174561439</v>
       </c>
       <c r="G25" t="n">
-        <v>-439.9708579235035</v>
+        <v>-31.42648985167882</v>
       </c>
       <c r="H25" t="n">
         <v>87</v>
@@ -1605,7 +1605,7 @@
         <v>9.515376593867099</v>
       </c>
       <c r="G26" t="n">
-        <v>-804.5066056322729</v>
+        <v>-33.52110856801137</v>
       </c>
       <c r="H26" t="n">
         <v>87</v>
@@ -1650,7 +1650,7 @@
         <v>3.897173500064501</v>
       </c>
       <c r="G27" t="n">
-        <v>-184.9399026613343</v>
+        <v>-36.98798053226686</v>
       </c>
       <c r="H27" t="n">
         <v>87</v>
@@ -1695,7 +1695,7 @@
         <v>6.586603111667807</v>
       </c>
       <c r="G28" t="n">
-        <v>-186.6441501543127</v>
+        <v>-37.32883003086253</v>
       </c>
       <c r="H28" t="n">
         <v>87</v>
@@ -1740,7 +1740,7 @@
         <v>0.3224843175145713</v>
       </c>
       <c r="G29" t="n">
-        <v>-185.1319981198243</v>
+        <v>-37.02639962396486</v>
       </c>
       <c r="H29" t="n">
         <v>87</v>
@@ -1785,7 +1785,7 @@
         <v>8.820620038469993</v>
       </c>
       <c r="G30" t="n">
-        <v>-403.4359108209827</v>
+        <v>-28.81685077292733</v>
       </c>
       <c r="H30" t="n">
         <v>87</v>
@@ -1830,7 +1830,7 @@
         <v>10.65952765089247</v>
       </c>
       <c r="G31" t="n">
-        <v>-408.388138182495</v>
+        <v>-29.17058129874964</v>
       </c>
       <c r="H31" t="n">
         <v>87</v>
@@ -1875,7 +1875,7 @@
         <v>12.92225312639015</v>
       </c>
       <c r="G32" t="n">
-        <v>-179.3076426236437</v>
+        <v>-35.86152852472874</v>
       </c>
       <c r="H32" t="n">
         <v>87</v>
@@ -1920,7 +1920,7 @@
         <v>10.5097240396306</v>
       </c>
       <c r="G33" t="n">
-        <v>-709.4428983145742</v>
+        <v>-35.47214491572871</v>
       </c>
       <c r="H33" t="n">
         <v>87</v>
@@ -1965,7 +1965,7 @@
         <v>11.11476749105106</v>
       </c>
       <c r="G34" t="n">
-        <v>-719.9779356840953</v>
+        <v>-35.99889678420477</v>
       </c>
       <c r="H34" t="n">
         <v>87</v>
@@ -2010,7 +2010,7 @@
         <v>8.527722349421067</v>
       </c>
       <c r="G35" t="n">
-        <v>-722.9836454052121</v>
+        <v>-36.1491822702606</v>
       </c>
       <c r="H35" t="n">
         <v>87</v>
@@ -2055,7 +2055,7 @@
         <v>8.688999517912123</v>
       </c>
       <c r="G36" t="n">
-        <v>-185.6188197452273</v>
+        <v>-37.12376394904545</v>
       </c>
       <c r="H36" t="n">
         <v>87</v>
@@ -2100,7 +2100,7 @@
         <v>19.74671801445167</v>
       </c>
       <c r="G37" t="n">
-        <v>-191.5325343500438</v>
+        <v>-23.94156679375547</v>
       </c>
       <c r="H37" t="n">
         <v>87</v>
@@ -2145,7 +2145,7 @@
         <v>6.792913964337708</v>
       </c>
       <c r="G38" t="n">
-        <v>-102.5301711896145</v>
+        <v>-34.1767237298715</v>
       </c>
       <c r="H38" t="n">
         <v>88</v>
@@ -2235,7 +2235,7 @@
         <v>20.01098682518023</v>
       </c>
       <c r="G40" t="n">
-        <v>-197.7069074804539</v>
+        <v>-24.71336343505674</v>
       </c>
       <c r="H40" t="n">
         <v>87</v>
@@ -2280,7 +2280,7 @@
         <v>-6.055665433125765</v>
       </c>
       <c r="G41" t="n">
-        <v>-4137.707839229434</v>
+        <v>-61.75683342133484</v>
       </c>
       <c r="H41" t="n">
         <v>87</v>
@@ -2325,7 +2325,7 @@
         <v>15.86678246881216</v>
       </c>
       <c r="G42" t="n">
-        <v>-540.8053476202862</v>
+        <v>-45.06711230169051</v>
       </c>
       <c r="H42" t="n">
         <v>87</v>
@@ -2370,7 +2370,7 @@
         <v>13.12724214294775</v>
       </c>
       <c r="G43" t="n">
-        <v>-646.0711681229492</v>
+        <v>-26.91963200512288</v>
       </c>
       <c r="H43" t="n">
         <v>87</v>
@@ -2415,7 +2415,7 @@
         <v>19.2286232221439</v>
       </c>
       <c r="G44" t="n">
-        <v>-1132.322432268375</v>
+        <v>-37.74408107561251</v>
       </c>
       <c r="H44" t="n">
         <v>87</v>
@@ -2460,7 +2460,7 @@
         <v>17.8016830163471</v>
       </c>
       <c r="G45" t="n">
-        <v>-1838.56282885586</v>
+        <v>-32.83147908671179</v>
       </c>
       <c r="H45" t="n">
         <v>87</v>
@@ -2505,7 +2505,7 @@
         <v>11.78870380634183</v>
       </c>
       <c r="G46" t="n">
-        <v>-1335.590783080489</v>
+        <v>-33.38976957701222</v>
       </c>
       <c r="H46" t="n">
         <v>87</v>
@@ -2550,7 +2550,7 @@
         <v>21.73164098005404</v>
       </c>
       <c r="G47" t="n">
-        <v>-144.1067860415215</v>
+        <v>-18.01334825519019</v>
       </c>
       <c r="H47" t="n">
         <v>88</v>
@@ -2595,7 +2595,7 @@
         <v>7.926683861369344</v>
       </c>
       <c r="G48" t="n">
-        <v>-647.4017326146475</v>
+        <v>-32.37008663073237</v>
       </c>
       <c r="H48" t="n">
         <v>87</v>
@@ -2640,7 +2640,7 @@
         <v>10.42856835744963</v>
       </c>
       <c r="G49" t="n">
-        <v>-173.1790042653138</v>
+        <v>-34.63580085306275</v>
       </c>
       <c r="H49" t="n">
         <v>87</v>
@@ -2685,7 +2685,7 @@
         <v>9.565654137439747</v>
       </c>
       <c r="G50" t="n">
-        <v>-177.9762288703952</v>
+        <v>-35.59524577407903</v>
       </c>
       <c r="H50" t="n">
         <v>87</v>
@@ -2730,7 +2730,7 @@
         <v>12.65323740949982</v>
       </c>
       <c r="G51" t="n">
-        <v>-879.0074546565523</v>
+        <v>-31.39312338059116</v>
       </c>
       <c r="H51" t="n">
         <v>87</v>
@@ -2775,7 +2775,7 @@
         <v>6.876931183789176</v>
       </c>
       <c r="G52" t="n">
-        <v>-716.8757956269243</v>
+        <v>-35.84378978134622</v>
       </c>
       <c r="H52" t="n">
         <v>87</v>
@@ -2820,7 +2820,7 @@
         <v>14.6016042618712</v>
       </c>
       <c r="G53" t="n">
-        <v>-1073.29010160827</v>
+        <v>-29.81361393356306</v>
       </c>
       <c r="H53" t="n">
         <v>87</v>
@@ -2865,7 +2865,7 @@
         <v>2.741028211725744</v>
       </c>
       <c r="G54" t="n">
-        <v>-632.9095098980176</v>
+        <v>-31.64547549490088</v>
       </c>
       <c r="H54" t="n">
         <v>87</v>
@@ -2910,7 +2910,7 @@
         <v>13.39501283582882</v>
       </c>
       <c r="G55" t="n">
-        <v>-1053.177255270723</v>
+        <v>-29.25492375752009</v>
       </c>
       <c r="H55" t="n">
         <v>87</v>
@@ -2955,7 +2955,7 @@
         <v>6.348269696591781</v>
       </c>
       <c r="G56" t="n">
-        <v>-726.1858434430932</v>
+        <v>-36.30929217215466</v>
       </c>
       <c r="H56" t="n">
         <v>87</v>
@@ -3000,7 +3000,7 @@
         <v>1.651646889616114</v>
       </c>
       <c r="G57" t="n">
-        <v>-761.6507698723765</v>
+        <v>-38.08253849361883</v>
       </c>
       <c r="H57" t="n">
         <v>87</v>
@@ -3045,7 +3045,7 @@
         <v>8.669813882990603</v>
       </c>
       <c r="G58" t="n">
-        <v>-1493.371588137134</v>
+        <v>-37.33428970342835</v>
       </c>
       <c r="H58" t="n">
         <v>87</v>
@@ -3090,7 +3090,7 @@
         <v>0.9468158984018835</v>
       </c>
       <c r="G59" t="n">
-        <v>-1230.266878446147</v>
+        <v>-51.26111993525611</v>
       </c>
       <c r="H59" t="n">
         <v>87</v>
@@ -3135,7 +3135,7 @@
         <v>16.24467568843643</v>
       </c>
       <c r="G60" t="n">
-        <v>-167.2329776889618</v>
+        <v>-20.90412221112022</v>
       </c>
       <c r="H60" t="n">
         <v>87</v>
@@ -3180,7 +3180,7 @@
         <v>12.03370521245074</v>
       </c>
       <c r="G61" t="n">
-        <v>-722.8359203328243</v>
+        <v>-36.14179601664122</v>
       </c>
       <c r="H61" t="n">
         <v>87</v>
@@ -3225,7 +3225,7 @@
         <v>12.14746123142425</v>
       </c>
       <c r="G62" t="n">
-        <v>-1767.672487575726</v>
+        <v>-31.56558013528083</v>
       </c>
       <c r="H62" t="n">
         <v>87</v>
@@ -3270,7 +3270,7 @@
         <v>5.171516888790909</v>
       </c>
       <c r="G63" t="n">
-        <v>-3924.356542172675</v>
+        <v>-44.59496070650767</v>
       </c>
       <c r="H63" t="n">
         <v>87</v>
@@ -3315,7 +3315,7 @@
         <v>19.52200769799984</v>
       </c>
       <c r="G64" t="n">
-        <v>-74.79576911202</v>
+        <v>-18.698942278005</v>
       </c>
       <c r="H64" t="n">
         <v>88</v>
@@ -3360,7 +3360,7 @@
         <v>15.29493110167907</v>
       </c>
       <c r="G65" t="n">
-        <v>-2356.774036850311</v>
+        <v>-29.45967546062889</v>
       </c>
       <c r="H65" t="n">
         <v>87</v>
@@ -3405,7 +3405,7 @@
         <v>11.15706407002315</v>
       </c>
       <c r="G66" t="n">
-        <v>-495.3665731243325</v>
+        <v>-41.28054776036104</v>
       </c>
       <c r="H66" t="n">
         <v>87</v>
@@ -3450,7 +3450,7 @@
         <v>-5.287248633119927</v>
       </c>
       <c r="G67" t="n">
-        <v>-1899.036113776873</v>
+        <v>-33.91135917458702</v>
       </c>
       <c r="H67" t="n">
         <v>87</v>
@@ -3495,7 +3495,7 @@
         <v>11.97892370876233</v>
       </c>
       <c r="G68" t="n">
-        <v>-424.9432495669838</v>
+        <v>-13.27947654896824</v>
       </c>
       <c r="H68" t="n">
         <v>84</v>
@@ -3540,7 +3540,7 @@
         <v>15.6728076704103</v>
       </c>
       <c r="G69" t="n">
-        <v>-188.895199194907</v>
+        <v>-23.61189989936338</v>
       </c>
       <c r="H69" t="n">
         <v>87</v>
@@ -3585,7 +3585,7 @@
         <v>11.97892370876233</v>
       </c>
       <c r="G70" t="n">
-        <v>-3981.052522568262</v>
+        <v>-124.4078913302582</v>
       </c>
       <c r="H70" t="n">
         <v>83</v>
@@ -3630,7 +3630,7 @@
         <v>11.97892370876233</v>
       </c>
       <c r="G71" t="n">
-        <v>-3567.597757033187</v>
+        <v>-111.4874299072871</v>
       </c>
       <c r="H71" t="n">
         <v>85</v>
@@ -3675,7 +3675,7 @@
         <v>14.37981275554606</v>
       </c>
       <c r="G72" t="n">
-        <v>-1085.247378795685</v>
+        <v>-36.17491262652285</v>
       </c>
       <c r="H72" t="n">
         <v>87</v>
@@ -3720,7 +3720,7 @@
         <v>-8.805939291487523</v>
       </c>
       <c r="G73" t="n">
-        <v>-1110.948942421993</v>
+        <v>-69.43430890137456</v>
       </c>
       <c r="H73" t="n">
         <v>87</v>
@@ -3765,7 +3765,7 @@
         <v>3.644867612597613</v>
       </c>
       <c r="G74" t="n">
-        <v>-132.2754140671005</v>
+        <v>-11.02295117225838</v>
       </c>
       <c r="H74" t="n">
         <v>87</v>
@@ -3810,7 +3810,7 @@
         <v>9.86474286769076</v>
       </c>
       <c r="G75" t="n">
-        <v>-504.9619762570557</v>
+        <v>-18.03435629489485</v>
       </c>
       <c r="H75" t="n">
         <v>87</v>
@@ -3855,7 +3855,7 @@
         <v>16.22096940973244</v>
       </c>
       <c r="G76" t="n">
-        <v>-210.225701045126</v>
+        <v>-26.27821263064075</v>
       </c>
       <c r="H76" t="n">
         <v>87</v>
@@ -3900,7 +3900,7 @@
         <v>12.63247841698307</v>
       </c>
       <c r="G77" t="n">
-        <v>-192.0036841592231</v>
+        <v>-24.00046051990288</v>
       </c>
       <c r="H77" t="n">
         <v>87</v>
@@ -3945,7 +3945,7 @@
         <v>13.02803257271935</v>
       </c>
       <c r="G78" t="n">
-        <v>-319.8464228135832</v>
+        <v>-26.6538685677986</v>
       </c>
       <c r="H78" t="n">
         <v>87</v>
@@ -3990,7 +3990,7 @@
         <v>16.29589297049844</v>
       </c>
       <c r="G79" t="n">
-        <v>-2551.610768262189</v>
+        <v>-31.89513460327736</v>
       </c>
       <c r="H79" t="n">
         <v>87</v>
@@ -4035,7 +4035,7 @@
         <v>11.49224901696388</v>
       </c>
       <c r="G80" t="n">
-        <v>-404.3770970679853</v>
+        <v>-28.88407836199895</v>
       </c>
       <c r="H80" t="n">
         <v>87</v>
@@ -4080,7 +4080,7 @@
         <v>12.57661562522831</v>
       </c>
       <c r="G81" t="n">
-        <v>-2469.200020234809</v>
+        <v>-30.86500025293512</v>
       </c>
       <c r="H81" t="n">
         <v>87</v>
@@ -4125,7 +4125,7 @@
         <v>14.59939498929582</v>
       </c>
       <c r="G82" t="n">
-        <v>-156.6044796125804</v>
+        <v>-19.57555995157255</v>
       </c>
       <c r="H82" t="n">
         <v>87</v>
@@ -4170,7 +4170,7 @@
         <v>14.07497622061901</v>
       </c>
       <c r="G83" t="n">
-        <v>-1071.509348528012</v>
+        <v>-35.71697828426706</v>
       </c>
       <c r="H83" t="n">
         <v>87</v>
@@ -4215,7 +4215,7 @@
         <v>15.96866751987036</v>
       </c>
       <c r="G84" t="n">
-        <v>-186.144298235758</v>
+        <v>-23.26803727946974</v>
       </c>
       <c r="H84" t="n">
         <v>87</v>
@@ -4260,7 +4260,7 @@
         <v>12.32765098569313</v>
       </c>
       <c r="G85" t="n">
-        <v>-120.5985214239989</v>
+        <v>-10.04987678533324</v>
       </c>
       <c r="H85" t="n">
         <v>88</v>
@@ -4305,7 +4305,7 @@
         <v>11.54674904400169</v>
       </c>
       <c r="G86" t="n">
-        <v>-405.604944164164</v>
+        <v>-28.97178172601171</v>
       </c>
       <c r="H86" t="n">
         <v>87</v>
@@ -4350,7 +4350,7 @@
         <v>16.10237501149364</v>
       </c>
       <c r="G87" t="n">
-        <v>-662.8323252467507</v>
+        <v>-33.14161626233754</v>
       </c>
       <c r="H87" t="n">
         <v>87</v>
@@ -4395,7 +4395,7 @@
         <v>15.75336413459036</v>
       </c>
       <c r="G88" t="n">
-        <v>-2526.175516493236</v>
+        <v>-31.57719395616544</v>
       </c>
       <c r="H88" t="n">
         <v>87</v>
@@ -4440,7 +4440,7 @@
         <v>3.246802306027917</v>
       </c>
       <c r="G89" t="n">
-        <v>-879.6163672354041</v>
+        <v>-43.9808183617702</v>
       </c>
       <c r="H89" t="n">
         <v>87</v>
@@ -4485,7 +4485,7 @@
         <v>19.18363122301929</v>
       </c>
       <c r="G90" t="n">
-        <v>-772.4876666386414</v>
+        <v>-27.58884523709434</v>
       </c>
       <c r="H90" t="n">
         <v>87</v>
@@ -4530,7 +4530,7 @@
         <v>14.58551882081348</v>
       </c>
       <c r="G91" t="n">
-        <v>-745.4317096847767</v>
+        <v>-14.33522518624571</v>
       </c>
       <c r="H91" t="n">
         <v>87</v>
@@ -4575,7 +4575,7 @@
         <v>16.51316941368032</v>
       </c>
       <c r="G92" t="n">
-        <v>-147.0388971876684</v>
+        <v>-29.40777943753368</v>
       </c>
       <c r="H92" t="n">
         <v>87</v>
@@ -4620,7 +4620,7 @@
         <v>8.709237899170516</v>
       </c>
       <c r="G93" t="n">
-        <v>-1139.148566102496</v>
+        <v>-35.59839269070302</v>
       </c>
       <c r="H93" t="n">
         <v>87</v>
@@ -4665,7 +4665,7 @@
         <v>15.80664109548973</v>
       </c>
       <c r="G94" t="n">
-        <v>-3309.08503038082</v>
+        <v>-37.60323898160023</v>
       </c>
       <c r="H94" t="n">
         <v>87</v>
@@ -4710,7 +4710,7 @@
         <v>13.87517545549936</v>
       </c>
       <c r="G95" t="n">
-        <v>-661.9462800334368</v>
+        <v>-33.09731400167184</v>
       </c>
       <c r="H95" t="n">
         <v>87</v>
@@ -4755,7 +4755,7 @@
         <v>13.30902822792875</v>
       </c>
       <c r="G96" t="n">
-        <v>-655.2826652348544</v>
+        <v>-32.76413326174272</v>
       </c>
       <c r="H96" t="n">
         <v>87</v>
@@ -4800,7 +4800,7 @@
         <v>10.56817572938078</v>
       </c>
       <c r="G97" t="n">
-        <v>-656.6204776231505</v>
+        <v>-32.83102388115752</v>
       </c>
       <c r="H97" t="n">
         <v>87</v>
@@ -4845,7 +4845,7 @@
         <v>11.96559982219208</v>
       </c>
       <c r="G98" t="n">
-        <v>-650.483656204629</v>
+        <v>-32.52418281023145</v>
       </c>
       <c r="H98" t="n">
         <v>87</v>
@@ -4890,7 +4890,7 @@
         <v>16.18066589778868</v>
       </c>
       <c r="G99" t="n">
-        <v>-650.7850217957023</v>
+        <v>-32.53925108978511</v>
       </c>
       <c r="H99" t="n">
         <v>87</v>
@@ -4935,7 +4935,7 @@
         <v>14.74290646578868</v>
       </c>
       <c r="G100" t="n">
-        <v>-655.7716620531577</v>
+        <v>-32.78858310265788</v>
       </c>
       <c r="H100" t="n">
         <v>87</v>
@@ -4980,7 +4980,7 @@
         <v>17.03888437639023</v>
       </c>
       <c r="G101" t="n">
-        <v>-616.2698532063869</v>
+        <v>-30.81349266031934</v>
       </c>
       <c r="H101" t="n">
         <v>87</v>
@@ -5025,7 +5025,7 @@
         <v>12.69292262306411</v>
       </c>
       <c r="G102" t="n">
-        <v>-318.269075833068</v>
+        <v>-26.522422986089</v>
       </c>
       <c r="H102" t="n">
         <v>87</v>
@@ -5070,7 +5070,7 @@
         <v>18.83109863025619</v>
       </c>
       <c r="G103" t="n">
-        <v>-2590.756077950437</v>
+        <v>-32.38445097438047</v>
       </c>
       <c r="H103" t="n">
         <v>87</v>
@@ -5115,7 +5115,7 @@
         <v>18.16337112353785</v>
       </c>
       <c r="G104" t="n">
-        <v>-190.9557112088899</v>
+        <v>-23.86946390111124</v>
       </c>
       <c r="H104" t="n">
         <v>87</v>
@@ -5160,7 +5160,7 @@
         <v>4.223162870729706</v>
       </c>
       <c r="G105" t="n">
-        <v>-1066.972860670953</v>
+        <v>-35.56576202236511</v>
       </c>
       <c r="H105" t="n">
         <v>87</v>
@@ -5205,7 +5205,7 @@
         <v>11.07444465832683</v>
       </c>
       <c r="G106" t="n">
-        <v>-2870.207561456212</v>
+        <v>-35.87759451820266</v>
       </c>
       <c r="H106" t="n">
         <v>87</v>
@@ -5250,7 +5250,7 @@
         <v>15.45152978654052</v>
       </c>
       <c r="G107" t="n">
-        <v>-181.1201606315539</v>
+        <v>-22.64002007894424</v>
       </c>
       <c r="H107" t="n">
         <v>87</v>
@@ -5295,7 +5295,7 @@
         <v>6.834580731998358</v>
       </c>
       <c r="G108" t="n">
-        <v>-293.5207616179201</v>
+        <v>-48.92012693632001</v>
       </c>
       <c r="H108" t="n">
         <v>87</v>
@@ -5340,7 +5340,7 @@
         <v>9.414516820353818</v>
       </c>
       <c r="G109" t="n">
-        <v>-1051.484333824173</v>
+        <v>-65.71777086401083</v>
       </c>
       <c r="H109" t="n">
         <v>87</v>
@@ -5385,7 +5385,7 @@
         <v>4.926845434851829</v>
       </c>
       <c r="G110" t="n">
-        <v>-278.9334414226365</v>
+        <v>-30.99260460251516</v>
       </c>
       <c r="H110" t="n">
         <v>88</v>
@@ -5430,7 +5430,7 @@
         <v>11.07205134859958</v>
       </c>
       <c r="G111" t="n">
-        <v>-398.4754985526246</v>
+        <v>-28.46253561090176</v>
       </c>
       <c r="H111" t="n">
         <v>87</v>
@@ -5475,7 +5475,7 @@
         <v>14.87158680620565</v>
       </c>
       <c r="G112" t="n">
-        <v>-151.1197931269381</v>
+        <v>-30.22395862538762</v>
       </c>
       <c r="H112" t="n">
         <v>87</v>
@@ -5520,7 +5520,7 @@
         <v>10.75817421596991</v>
       </c>
       <c r="G113" t="n">
-        <v>-662.8115681172819</v>
+        <v>-33.1405784058641</v>
       </c>
       <c r="H113" t="n">
         <v>87</v>
@@ -5565,7 +5565,7 @@
         <v>15.41167795475325</v>
       </c>
       <c r="G114" t="n">
-        <v>-192.7382082737886</v>
+        <v>-24.09227603422358</v>
       </c>
       <c r="H114" t="n">
         <v>87</v>
@@ -5610,7 +5610,7 @@
         <v>-1.862887256628939</v>
       </c>
       <c r="G115" t="n">
-        <v>-409.5767730273667</v>
+        <v>-45.50853033637408</v>
       </c>
       <c r="H115" t="n">
         <v>87</v>
@@ -5655,7 +5655,7 @@
         <v>21.95593646510948</v>
       </c>
       <c r="G116" t="n">
-        <v>-82.82506173535228</v>
+        <v>-20.70626543383807</v>
       </c>
       <c r="H116" t="n">
         <v>88</v>
@@ -5700,7 +5700,7 @@
         <v>8.692741461596764</v>
       </c>
       <c r="G117" t="n">
-        <v>-75.3334764248505</v>
+        <v>-18.83336910621263</v>
       </c>
       <c r="H117" t="n">
         <v>87</v>
@@ -5745,7 +5745,7 @@
         <v>10.09272549676122</v>
       </c>
       <c r="G118" t="n">
-        <v>-180.7254739485267</v>
+        <v>-36.14509478970533</v>
       </c>
       <c r="H118" t="n">
         <v>87</v>
@@ -5790,7 +5790,7 @@
         <v>11.83859620530502</v>
       </c>
       <c r="G119" t="n">
-        <v>-92.28413734275537</v>
+        <v>-23.07103433568884</v>
       </c>
       <c r="H119" t="n">
         <v>87</v>
@@ -5835,7 +5835,7 @@
         <v>10.98011173316974</v>
       </c>
       <c r="G120" t="n">
-        <v>-395.7152328553078</v>
+        <v>-28.26537377537913</v>
       </c>
       <c r="H120" t="n">
         <v>87</v>
@@ -5880,7 +5880,7 @@
         <v>15.29746612400971</v>
       </c>
       <c r="G121" t="n">
-        <v>-150.2381184025318</v>
+        <v>-30.04762368050637</v>
       </c>
       <c r="H121" t="n">
         <v>87</v>
@@ -5925,7 +5925,7 @@
         <v>10.82576286667492</v>
       </c>
       <c r="G122" t="n">
-        <v>-661.70441950554</v>
+        <v>-33.085220975277</v>
       </c>
       <c r="H122" t="n">
         <v>87</v>
@@ -5970,7 +5970,7 @@
         <v>9.293078007973538</v>
       </c>
       <c r="G123" t="n">
-        <v>-497.2407344914946</v>
+        <v>-41.43672787429121</v>
       </c>
       <c r="H123" t="n">
         <v>87</v>
@@ -6015,7 +6015,7 @@
         <v>11.32147282158181</v>
       </c>
       <c r="G124" t="n">
-        <v>-276.9848647784129</v>
+        <v>-46.16414412973549</v>
       </c>
       <c r="H124" t="n">
         <v>87</v>
@@ -6060,7 +6060,7 @@
         <v>12.94444751324791</v>
       </c>
       <c r="G125" t="n">
-        <v>-1057.898941934569</v>
+        <v>-35.26329806448565</v>
       </c>
       <c r="H125" t="n">
         <v>87</v>
@@ -6105,7 +6105,7 @@
         <v>0.4364275976059835</v>
       </c>
       <c r="G126" t="n">
-        <v>-3501.956371968005</v>
+        <v>-35.01956371968004</v>
       </c>
       <c r="H126" t="n">
         <v>87</v>
@@ -6150,7 +6150,7 @@
         <v>11.38391685233449</v>
       </c>
       <c r="G127" t="n">
-        <v>-402.4480628020721</v>
+        <v>-28.746290200148</v>
       </c>
       <c r="H127" t="n">
         <v>87</v>
@@ -6195,7 +6195,7 @@
         <v>14.52469475782423</v>
       </c>
       <c r="G128" t="n">
-        <v>-913.2718405274597</v>
+        <v>-30.44239468424866</v>
       </c>
       <c r="H128" t="n">
         <v>87</v>
@@ -6240,7 +6240,7 @@
         <v>10.25203530105554</v>
       </c>
       <c r="G129" t="n">
-        <v>-78.17461034971214</v>
+        <v>-19.54365258742803</v>
       </c>
       <c r="H129" t="n">
         <v>87</v>
@@ -6285,7 +6285,7 @@
         <v>11.99224759533257</v>
       </c>
       <c r="G130" t="n">
-        <v>-269.8079206891012</v>
+        <v>-44.96798678151686</v>
       </c>
       <c r="H130" t="n">
         <v>87</v>
@@ -6330,7 +6330,7 @@
         <v>14.90335040175579</v>
       </c>
       <c r="G131" t="n">
-        <v>-392.6864028231136</v>
+        <v>-28.04902877307954</v>
       </c>
       <c r="H131" t="n">
         <v>87</v>
@@ -6375,7 +6375,7 @@
         <v>-1.83178341544144</v>
       </c>
       <c r="G132" t="n">
-        <v>-518.6364709126113</v>
+        <v>-25.93182354563057</v>
       </c>
       <c r="H132" t="n">
         <v>87</v>
@@ -6420,7 +6420,7 @@
         <v>-0.4691385797749499</v>
       </c>
       <c r="G133" t="n">
-        <v>-182.8036370711769</v>
+        <v>-36.56072741423539</v>
       </c>
       <c r="H133" t="n">
         <v>87</v>
@@ -6465,7 +6465,7 @@
         <v>7.257440483103506</v>
       </c>
       <c r="G134" t="n">
-        <v>-703.6749742021906</v>
+        <v>-35.18374871010953</v>
       </c>
       <c r="H134" t="n">
         <v>87</v>
@@ -6510,7 +6510,7 @@
         <v>6.1983982871848</v>
       </c>
       <c r="G135" t="n">
-        <v>-441.9806268495833</v>
+        <v>-31.57004477497023</v>
       </c>
       <c r="H135" t="n">
         <v>87</v>
@@ -6555,7 +6555,7 @@
         <v>16.64639859713828</v>
       </c>
       <c r="G136" t="n">
-        <v>-1568.284954219487</v>
+        <v>-39.20712385548718</v>
       </c>
       <c r="H136" t="n">
         <v>87</v>
@@ -6600,7 +6600,7 @@
         <v>-23.05567157245508</v>
       </c>
       <c r="G137" t="n">
-        <v>-732.960043467657</v>
+        <v>-36.64800217338285</v>
       </c>
       <c r="H137" t="n">
         <v>87</v>
@@ -6645,7 +6645,7 @@
         <v>11.48080112895222</v>
       </c>
       <c r="G138" t="n">
-        <v>-724.3344253051387</v>
+        <v>-36.21672126525694</v>
       </c>
       <c r="H138" t="n">
         <v>87</v>
@@ -6690,7 +6690,7 @@
         <v>14.3054639897824</v>
       </c>
       <c r="G139" t="n">
-        <v>-383.5860582798898</v>
+        <v>-27.39900416284927</v>
       </c>
       <c r="H139" t="n">
         <v>87</v>
@@ -6735,7 +6735,7 @@
         <v>4.965246812817715</v>
       </c>
       <c r="G140" t="n">
-        <v>-450.7163906025439</v>
+        <v>-32.19402790018171</v>
       </c>
       <c r="H140" t="n">
         <v>87</v>
@@ -6780,7 +6780,7 @@
         <v>37.3524945037901</v>
       </c>
       <c r="G141" t="n">
-        <v>-716.6606458886365</v>
+        <v>-35.83303229443182</v>
       </c>
       <c r="H141" t="n">
         <v>87</v>
@@ -6825,7 +6825,7 @@
         <v>11.61134175797678</v>
       </c>
       <c r="G142" t="n">
-        <v>-427.3630529558874</v>
+        <v>-30.52593235399195</v>
       </c>
       <c r="H142" t="n">
         <v>87</v>
@@ -6870,7 +6870,7 @@
         <v>11.60656275966077</v>
       </c>
       <c r="G143" t="n">
-        <v>-442.7809721800561</v>
+        <v>-31.62721229857544</v>
       </c>
       <c r="H143" t="n">
         <v>87</v>
@@ -6915,7 +6915,7 @@
         <v>8.880294477012001</v>
       </c>
       <c r="G144" t="n">
-        <v>-446.5183315763138</v>
+        <v>-31.89416654116527</v>
       </c>
       <c r="H144" t="n">
         <v>87</v>
@@ -6960,7 +6960,7 @@
         <v>6.223374401796821</v>
       </c>
       <c r="G145" t="n">
-        <v>-4634.362593606023</v>
+        <v>-38.6196882800502</v>
       </c>
       <c r="H145" t="n">
         <v>87</v>
@@ -7005,7 +7005,7 @@
         <v>16.25401085446282</v>
       </c>
       <c r="G146" t="n">
-        <v>-1533.278534598094</v>
+        <v>-31.94330280412696</v>
       </c>
       <c r="H146" t="n">
         <v>87</v>
@@ -7050,7 +7050,7 @@
         <v>5.042384732262713</v>
       </c>
       <c r="G147" t="n">
-        <v>-1042.195535195121</v>
+        <v>-34.7398511731707</v>
       </c>
       <c r="H147" t="n">
         <v>87</v>
@@ -7095,7 +7095,7 @@
         <v>1.969969444817323</v>
       </c>
       <c r="G148" t="n">
-        <v>-1250.950017857474</v>
+        <v>-31.27375044643686</v>
       </c>
       <c r="H148" t="n">
         <v>87</v>
@@ -7140,7 +7140,7 @@
         <v>9.504710828478689</v>
       </c>
       <c r="G149" t="n">
-        <v>-650.3443333382857</v>
+        <v>-32.51721666691428</v>
       </c>
       <c r="H149" t="n">
         <v>87</v>
@@ -7185,7 +7185,7 @@
         <v>12.45119699628211</v>
       </c>
       <c r="G150" t="n">
-        <v>-408.6269531921024</v>
+        <v>-29.1876395137216</v>
       </c>
       <c r="H150" t="n">
         <v>87</v>
@@ -7230,7 +7230,7 @@
         <v>14.57034923573437</v>
       </c>
       <c r="G151" t="n">
-        <v>-406.1429294205735</v>
+        <v>-29.01020924432668</v>
       </c>
       <c r="H151" t="n">
         <v>87</v>
@@ -7275,7 +7275,7 @@
         <v>15.37642576845103</v>
       </c>
       <c r="G152" t="n">
-        <v>-401.1564693971799</v>
+        <v>-28.65403352836999</v>
       </c>
       <c r="H152" t="n">
         <v>87</v>
@@ -7320,7 +7320,7 @@
         <v>4.79849987569956</v>
       </c>
       <c r="G153" t="n">
-        <v>-187.414454078348</v>
+        <v>-37.48289081566959</v>
       </c>
       <c r="H153" t="n">
         <v>87</v>
@@ -7365,7 +7365,7 @@
         <v>2.399341419532863</v>
       </c>
       <c r="G154" t="n">
-        <v>-1243.481142710901</v>
+        <v>-51.81171427962087</v>
       </c>
       <c r="H154" t="n">
         <v>87</v>
@@ -7410,7 +7410,7 @@
         <v>7.287515916658765</v>
       </c>
       <c r="G155" t="n">
-        <v>-649.884014025921</v>
+        <v>-32.49420070129605</v>
       </c>
       <c r="H155" t="n">
         <v>87</v>
@@ -7455,7 +7455,7 @@
         <v>10.86675790403808</v>
       </c>
       <c r="G156" t="n">
-        <v>-702.146596403716</v>
+        <v>-35.1073298201858</v>
       </c>
       <c r="H156" t="n">
         <v>87</v>
@@ -7500,7 +7500,7 @@
         <v>11.09490760377686</v>
       </c>
       <c r="G157" t="n">
-        <v>-182.5719141509459</v>
+        <v>-36.51438283018918</v>
       </c>
       <c r="H157" t="n">
         <v>87</v>
@@ -7545,7 +7545,7 @@
         <v>-8.800676069193702</v>
       </c>
       <c r="G158" t="n">
-        <v>-1043.229630034403</v>
+        <v>-43.46790125143344</v>
       </c>
       <c r="H158" t="n">
         <v>87</v>
@@ -7590,7 +7590,7 @@
         <v>16.03992679437992</v>
       </c>
       <c r="G159" t="n">
-        <v>-688.5790512120122</v>
+        <v>-34.42895256060061</v>
       </c>
       <c r="H159" t="n">
         <v>87</v>
@@ -7635,7 +7635,7 @@
         <v>12.31097088869684</v>
       </c>
       <c r="G160" t="n">
-        <v>-282.4889622854736</v>
+        <v>-47.0814937142456</v>
       </c>
       <c r="H160" t="n">
         <v>87</v>
@@ -7680,7 +7680,7 @@
         <v>15.78917120196562</v>
       </c>
       <c r="G161" t="n">
-        <v>-2573.929799269634</v>
+        <v>-32.17412249087042</v>
       </c>
       <c r="H161" t="n">
         <v>87</v>
@@ -7725,7 +7725,7 @@
         <v>7.008233717418752</v>
       </c>
       <c r="G162" t="n">
-        <v>-806.4016099983726</v>
+        <v>-57.60011499988376</v>
       </c>
       <c r="H162" t="n">
         <v>87</v>
@@ -7770,7 +7770,7 @@
         <v>13.34968022952277</v>
       </c>
       <c r="G163" t="n">
-        <v>-3518.111142724774</v>
+        <v>-39.97853571278153</v>
       </c>
       <c r="H163" t="n">
         <v>87</v>
@@ -7815,7 +7815,7 @@
         <v>14.40930931692454</v>
       </c>
       <c r="G164" t="n">
-        <v>-2575.497409452259</v>
+        <v>-32.19371761815324</v>
       </c>
       <c r="H164" t="n">
         <v>87</v>
@@ -7860,7 +7860,7 @@
         <v>15.48321714782841</v>
       </c>
       <c r="G165" t="n">
-        <v>-165.1138474816257</v>
+        <v>-20.63923093520322</v>
       </c>
       <c r="H165" t="n">
         <v>87</v>
@@ -7905,7 +7905,7 @@
         <v>14.8305646652595</v>
       </c>
       <c r="G166" t="n">
-        <v>-95.52994485268722</v>
+        <v>-23.88248621317181</v>
       </c>
       <c r="H166" t="n">
         <v>87</v>
@@ -7950,7 +7950,7 @@
         <v>20.9629780426437</v>
       </c>
       <c r="G167" t="n">
-        <v>-80.68933472258121</v>
+        <v>-20.1723336806453</v>
       </c>
       <c r="H167" t="n">
         <v>88</v>
@@ -7995,7 +7995,7 @@
         <v>2.57389885611642</v>
       </c>
       <c r="G168" t="n">
-        <v>-276.9137070589196</v>
+        <v>-27.69137070589196</v>
       </c>
       <c r="H168" t="n">
         <v>88</v>
@@ -8040,7 +8040,7 @@
         <v>8.843086198732404</v>
       </c>
       <c r="G169" t="n">
-        <v>-678.9804634488494</v>
+        <v>-33.94902317244247</v>
       </c>
       <c r="H169" t="n">
         <v>87</v>
@@ -8085,7 +8085,7 @@
         <v>9.365786937033809</v>
       </c>
       <c r="G170" t="n">
-        <v>-895.894567255433</v>
+        <v>-31.99623454483689</v>
       </c>
       <c r="H170" t="n">
         <v>87</v>
@@ -8130,7 +8130,7 @@
         <v>2.841627625085777</v>
       </c>
       <c r="G171" t="n">
-        <v>-2397.035010252683</v>
+        <v>-35.25051485665711</v>
       </c>
       <c r="H171" t="n">
         <v>87</v>
@@ -8175,7 +8175,7 @@
         <v>17.74524308058001</v>
       </c>
       <c r="G172" t="n">
-        <v>-1523.057244409665</v>
+        <v>-38.07643111024163</v>
       </c>
       <c r="H172" t="n">
         <v>87</v>
@@ -8220,7 +8220,7 @@
         <v>0.6549023837945214</v>
       </c>
       <c r="G173" t="n">
-        <v>-750.0759614341813</v>
+        <v>-37.50379807170906</v>
       </c>
       <c r="H173" t="n">
         <v>87</v>
@@ -8265,7 +8265,7 @@
         <v>8.724150244178947</v>
       </c>
       <c r="G174" t="n">
-        <v>-3902.501968404761</v>
+        <v>-44.34661327732683</v>
       </c>
       <c r="H174" t="n">
         <v>87</v>
@@ -8310,7 +8310,7 @@
         <v>20.48844292924497</v>
       </c>
       <c r="G175" t="n">
-        <v>-1544.636729379552</v>
+        <v>-27.58279873892058</v>
       </c>
       <c r="H175" t="n">
         <v>88</v>
@@ -8355,7 +8355,7 @@
         <v>7.496646130272039</v>
       </c>
       <c r="G176" t="n">
-        <v>-1423.269391290985</v>
+        <v>-35.58173478227462</v>
       </c>
       <c r="H176" t="n">
         <v>87</v>
@@ -8400,7 +8400,7 @@
         <v>10.40502885416976</v>
       </c>
       <c r="G177" t="n">
-        <v>-683.0751145235988</v>
+        <v>-34.15375572617994</v>
       </c>
       <c r="H177" t="n">
         <v>87</v>
@@ -8445,7 +8445,7 @@
         <v>7.578987374987769</v>
       </c>
       <c r="G178" t="n">
-        <v>-1424.257800241215</v>
+        <v>-35.60644500603038</v>
       </c>
       <c r="H178" t="n">
         <v>87</v>
@@ -8490,7 +8490,7 @@
         <v>10.46538126140717</v>
       </c>
       <c r="G179" t="n">
-        <v>-685.3802975942033</v>
+        <v>-34.26901487971016</v>
       </c>
       <c r="H179" t="n">
         <v>87</v>
@@ -8535,7 +8535,7 @@
         <v>8.609178690970637</v>
       </c>
       <c r="G180" t="n">
-        <v>-1417.997106736015</v>
+        <v>-35.44992766840037</v>
       </c>
       <c r="H180" t="n">
         <v>87</v>
@@ -8580,7 +8580,7 @@
         <v>10.36362466406775</v>
       </c>
       <c r="G181" t="n">
-        <v>-680.2636742687662</v>
+        <v>-34.01318371343831</v>
       </c>
       <c r="H181" t="n">
         <v>87</v>
@@ -8625,7 +8625,7 @@
         <v>3.736210023984296</v>
       </c>
       <c r="G182" t="n">
-        <v>-1792.031180253049</v>
+        <v>-32.00055679023301</v>
       </c>
       <c r="H182" t="n">
         <v>87</v>
@@ -8670,7 +8670,7 @@
         <v>14.42112484688565</v>
       </c>
       <c r="G183" t="n">
-        <v>-990.2237314090503</v>
+        <v>-33.00745771363501</v>
       </c>
       <c r="H183" t="n">
         <v>87</v>
@@ -8715,7 +8715,7 @@
         <v>22.91910830718785</v>
       </c>
       <c r="G184" t="n">
-        <v>-160.850466578575</v>
+        <v>-20.10630832232187</v>
       </c>
       <c r="H184" t="n">
         <v>88</v>
@@ -8760,7 +8760,7 @@
         <v>7.531115260990568</v>
       </c>
       <c r="G185" t="n">
-        <v>-1420.498153250185</v>
+        <v>-35.51245383125462</v>
       </c>
       <c r="H185" t="n">
         <v>87</v>
@@ -8805,7 +8805,7 @@
         <v>10.41311027771273</v>
       </c>
       <c r="G186" t="n">
-        <v>-681.439923665245</v>
+        <v>-34.07199618326225</v>
       </c>
       <c r="H186" t="n">
         <v>87</v>
@@ -8850,7 +8850,7 @@
         <v>5.12516377827888</v>
       </c>
       <c r="G187" t="n">
-        <v>-3913.959007547109</v>
+        <v>-44.47680690394442</v>
       </c>
       <c r="H187" t="n">
         <v>87</v>
@@ -8895,7 +8895,7 @@
         <v>7.514838663258059</v>
       </c>
       <c r="G188" t="n">
-        <v>-1423.51387589979</v>
+        <v>-35.58784689749474</v>
       </c>
       <c r="H188" t="n">
         <v>87</v>
@@ -8940,7 +8940,7 @@
         <v>-1.585859030433745</v>
       </c>
       <c r="G189" t="n">
-        <v>-4905.005998145802</v>
+        <v>-57.03495346681165</v>
       </c>
       <c r="H189" t="n">
         <v>87</v>
@@ -8985,7 +8985,7 @@
         <v>10.67360225253062</v>
       </c>
       <c r="G190" t="n">
-        <v>-1052.37095775339</v>
+        <v>-40.47580606743809</v>
       </c>
       <c r="H190" t="n">
         <v>87</v>
@@ -9030,7 +9030,7 @@
         <v>11.83196556717975</v>
       </c>
       <c r="G191" t="n">
-        <v>-332.8354695843322</v>
+        <v>-33.28354695843322</v>
       </c>
       <c r="H191" t="n">
         <v>87</v>
@@ -9075,7 +9075,7 @@
         <v>17.24000592169813</v>
       </c>
       <c r="G192" t="n">
-        <v>-1481.805691023788</v>
+        <v>-37.0451422755947</v>
       </c>
       <c r="H192" t="n">
         <v>87</v>
@@ -9120,7 +9120,7 @@
         <v>17.05796030706836</v>
       </c>
       <c r="G193" t="n">
-        <v>-1459.616830546363</v>
+        <v>-36.49042076365907</v>
       </c>
       <c r="H193" t="n">
         <v>87</v>
@@ -9165,7 +9165,7 @@
         <v>7.398844975528144</v>
       </c>
       <c r="G194" t="n">
-        <v>-1424.679848041712</v>
+        <v>-35.6169962010428</v>
       </c>
       <c r="H194" t="n">
         <v>87</v>
@@ -9210,7 +9210,7 @@
         <v>10.44584191545162</v>
       </c>
       <c r="G195" t="n">
-        <v>-689.2165603484071</v>
+        <v>-34.46082801742035</v>
       </c>
       <c r="H195" t="n">
         <v>87</v>
@@ -9255,7 +9255,7 @@
         <v>12.78862444257534</v>
       </c>
       <c r="G196" t="n">
-        <v>-1747.964439240916</v>
+        <v>-31.21365070073065</v>
       </c>
       <c r="H196" t="n">
         <v>87</v>
@@ -9300,7 +9300,7 @@
         <v>9.06661456446461</v>
       </c>
       <c r="G197" t="n">
-        <v>-871.1548145011932</v>
+        <v>-43.55774072505966</v>
       </c>
       <c r="H197" t="n">
         <v>87</v>
@@ -9345,7 +9345,7 @@
         <v>14.78554466175928</v>
       </c>
       <c r="G198" t="n">
-        <v>-268.6490697120228</v>
+        <v>-44.7748449520038</v>
       </c>
       <c r="H198" t="n">
         <v>87</v>
@@ -9390,7 +9390,7 @@
         <v>12.70653968661238</v>
       </c>
       <c r="G199" t="n">
-        <v>-3446.426571532708</v>
+        <v>-39.16393831287168</v>
       </c>
       <c r="H199" t="n">
         <v>87</v>
@@ -9435,7 +9435,7 @@
         <v>12.57996609409998</v>
       </c>
       <c r="G200" t="n">
-        <v>-681.8352960223759</v>
+        <v>-34.0917648011188</v>
       </c>
       <c r="H200" t="n">
         <v>87</v>
@@ -9480,7 +9480,7 @@
         <v>7.623952465316564</v>
       </c>
       <c r="G201" t="n">
-        <v>-1418.120418752285</v>
+        <v>-35.45301046880711</v>
       </c>
       <c r="H201" t="n">
         <v>87</v>
@@ -9525,7 +9525,7 @@
         <v>10.55672032452999</v>
       </c>
       <c r="G202" t="n">
-        <v>-676.4453622081401</v>
+        <v>-33.822268110407</v>
       </c>
       <c r="H202" t="n">
         <v>87</v>
@@ -9570,7 +9570,7 @@
         <v>8.891047942456183</v>
       </c>
       <c r="G203" t="n">
-        <v>-113.1034037916621</v>
+        <v>-9.425283649305173</v>
       </c>
       <c r="H203" t="n">
         <v>89</v>
@@ -9615,7 +9615,7 @@
         <v>-12.34258276638579</v>
       </c>
       <c r="G204" t="n">
-        <v>-3202.494163446984</v>
+        <v>-94.19100480726424</v>
       </c>
       <c r="H204" t="n">
         <v>83</v>
@@ -9660,7 +9660,7 @@
         <v>11.77696027679629</v>
       </c>
       <c r="G205" t="n">
-        <v>-670.2593825893637</v>
+        <v>-33.51296912946818</v>
       </c>
       <c r="H205" t="n">
         <v>87</v>
@@ -9705,7 +9705,7 @@
         <v>8.52066733818938</v>
       </c>
       <c r="G206" t="n">
-        <v>-1412.571449637729</v>
+        <v>-35.31428624094322</v>
       </c>
       <c r="H206" t="n">
         <v>87</v>
@@ -9750,7 +9750,7 @@
         <v>10.46084413160131</v>
       </c>
       <c r="G207" t="n">
-        <v>-675.003007371588</v>
+        <v>-33.7501503685794</v>
       </c>
       <c r="H207" t="n">
         <v>87</v>
@@ -9795,7 +9795,7 @@
         <v>-12.78643632310234</v>
       </c>
       <c r="G208" t="n">
-        <v>-3190.361592116282</v>
+        <v>-93.8341644740083</v>
       </c>
       <c r="H208" t="n">
         <v>83</v>
@@ -9840,7 +9840,7 @@
         <v>7.563981718543675</v>
       </c>
       <c r="G209" t="n">
-        <v>-1419.427717392216</v>
+        <v>-35.48569293480539</v>
       </c>
       <c r="H209" t="n">
         <v>87</v>
@@ -9885,7 +9885,7 @@
         <v>10.43553780722969</v>
       </c>
       <c r="G210" t="n">
-        <v>-678.1471072006465</v>
+        <v>-33.90735536003233</v>
       </c>
       <c r="H210" t="n">
         <v>87</v>
@@ -9930,7 +9930,7 @@
         <v>9.321527276927053</v>
       </c>
       <c r="G211" t="n">
-        <v>-999.5875636467322</v>
+        <v>-33.31958545489108</v>
       </c>
       <c r="H211" t="n">
         <v>87</v>
@@ -9975,7 +9975,7 @@
         <v>-0.3975568573342567</v>
       </c>
       <c r="G212" t="n">
-        <v>-402.814667988029</v>
+        <v>-33.56788899900242</v>
       </c>
       <c r="H212" t="n">
         <v>87</v>
@@ -10020,7 +10020,7 @@
         <v>7.431509855536475</v>
       </c>
       <c r="G213" t="n">
-        <v>-1421.718774576849</v>
+        <v>-35.54296936442124</v>
       </c>
       <c r="H213" t="n">
         <v>87</v>
@@ -10065,7 +10065,7 @@
         <v>17.92468059695952</v>
       </c>
       <c r="G214" t="n">
-        <v>-684.3970721552239</v>
+        <v>-34.21985360776119</v>
       </c>
       <c r="H214" t="n">
         <v>87</v>
@@ -10110,7 +10110,7 @@
         <v>16.16980573172836</v>
       </c>
       <c r="G215" t="n">
-        <v>-1051.27170749417</v>
+        <v>-35.04239024980568</v>
       </c>
       <c r="H215" t="n">
         <v>87</v>
@@ -10155,7 +10155,7 @@
         <v>-4.898513948778488</v>
       </c>
       <c r="G216" t="n">
-        <v>-1259.228516857661</v>
+        <v>-39.35089115180192</v>
       </c>
       <c r="H216" t="n">
         <v>87</v>
@@ -10200,7 +10200,7 @@
         <v>14.68437767723979</v>
       </c>
       <c r="G217" t="n">
-        <v>-1806.019889027586</v>
+        <v>-41.04590656880878</v>
       </c>
       <c r="H217" t="n">
         <v>87</v>
@@ -10245,7 +10245,7 @@
         <v>-5.624647139158788</v>
       </c>
       <c r="G218" t="n">
-        <v>-4338.575395339352</v>
+        <v>-49.30199312885627</v>
       </c>
       <c r="H218" t="n">
         <v>87</v>
@@ -10290,7 +10290,7 @@
         <v>7.386537343037568</v>
       </c>
       <c r="G219" t="n">
-        <v>-1423.588551676167</v>
+        <v>-35.58971379190418</v>
       </c>
       <c r="H219" t="n">
         <v>87</v>
@@ -10335,7 +10335,7 @@
         <v>15.30012090301311</v>
       </c>
       <c r="G220" t="n">
-        <v>-1070.255618291461</v>
+        <v>-35.67518727638205</v>
       </c>
       <c r="H220" t="n">
         <v>87</v>
@@ -10380,7 +10380,7 @@
         <v>-7.851262176983437</v>
       </c>
       <c r="G221" t="n">
-        <v>-1278.708095680477</v>
+        <v>-39.9596279900149</v>
       </c>
       <c r="H221" t="n">
         <v>87</v>
@@ -10425,7 +10425,7 @@
         <v>14.39788179607763</v>
       </c>
       <c r="G222" t="n">
-        <v>-925.019001766282</v>
+        <v>-42.04631826210373</v>
       </c>
       <c r="H222" t="n">
         <v>87</v>
@@ -10470,7 +10470,7 @@
         <v>0.3212686741655322</v>
       </c>
       <c r="G223" t="n">
-        <v>-1201.489266723702</v>
+        <v>-42.91033095441792</v>
       </c>
       <c r="H223" t="n">
         <v>87</v>
@@ -10515,7 +10515,7 @@
         <v>-1.565994023966407</v>
       </c>
       <c r="G224" t="n">
-        <v>-1497.068794319018</v>
+        <v>-44.03143512702994</v>
       </c>
       <c r="H224" t="n">
         <v>87</v>
@@ -10560,7 +10560,7 @@
         <v>-12.46702007568821</v>
       </c>
       <c r="G225" t="n">
-        <v>-1960.406861073423</v>
+        <v>-51.58965423877429</v>
       </c>
       <c r="H225" t="n">
         <v>87</v>
@@ -10605,7 +10605,7 @@
         <v>11.94068145695785</v>
       </c>
       <c r="G226" t="n">
-        <v>-2059.225053940771</v>
+        <v>-44.76576204219067</v>
       </c>
       <c r="H226" t="n">
         <v>87</v>
@@ -10650,7 +10650,7 @@
         <v>9.779242118562511</v>
       </c>
       <c r="G227" t="n">
-        <v>-286.6875445978383</v>
+        <v>-47.78125743297304</v>
       </c>
       <c r="H227" t="n">
         <v>87</v>
@@ -10695,7 +10695,7 @@
         <v>10.39327840988674</v>
       </c>
       <c r="G228" t="n">
-        <v>-684.0478611509031</v>
+        <v>-34.20239305754516</v>
       </c>
       <c r="H228" t="n">
         <v>87</v>
@@ -10740,7 +10740,7 @@
         <v>7.361180849620142</v>
       </c>
       <c r="G229" t="n">
-        <v>-1424.019987213344</v>
+        <v>-35.6004996803336</v>
       </c>
       <c r="H229" t="n">
         <v>87</v>

</xml_diff>